<commit_message>
Minor changes to template excel file for improved workflow
</commit_message>
<xml_diff>
--- a/Schema_to_Excel/temoa_schema.xlsx
+++ b/Schema_to_Excel/temoa_schema.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ianda\Documents\University\TEMOA project\TEMOA_Excel_SQLite_Conversion\Schema_to_Excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DB763C-CA8B-47D8-AE23-BFDE2DE63DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="CapacityCredit" sheetId="1" r:id="rId1"/>
@@ -68,7 +62,7 @@
     <sheet name="time_periods" sheetId="53" r:id="rId53"/>
     <sheet name="time_season" sheetId="54" r:id="rId54"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -405,8 +399,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -443,830 +437,822 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H101" totalsRowShown="0">
-  <autoFilter ref="A1:H101" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H101" totalsRowShown="0">
+  <autoFilter ref="A1:H101"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="periods"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="tech"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="vintage"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="cf_tech"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="cf_tech_notes"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="source"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="periods"/>
+    <tableColumn id="3" name="tech"/>
+    <tableColumn id="4" name="vintage"/>
+    <tableColumn id="5" name="cf_tech"/>
+    <tableColumn id="6" name="cf_tech_notes"/>
+    <tableColumn id="7" name="source"/>
+    <tableColumn id="8" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Table10" displayName="Table10" ref="A1:G101" totalsRowShown="0">
-  <autoFilter ref="A1:G101" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A1:G101" totalsRowShown="0">
+  <autoFilter ref="A1:G101"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="tech"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="vintage"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="tech_rate"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="tech_rate_notes"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="source"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="tech"/>
+    <tableColumn id="3" name="vintage"/>
+    <tableColumn id="4" name="tech_rate"/>
+    <tableColumn id="5" name="tech_rate_notes"/>
+    <tableColumn id="6" name="source"/>
+    <tableColumn id="7" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Table11" displayName="Table11" ref="A1:I101" totalsRowShown="0">
-  <autoFilter ref="A1:I101" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A1:I101" totalsRowShown="0">
+  <autoFilter ref="A1:I101"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="input_comm"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="tech"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="vintage"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="output_comm"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="efficiency"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0A00-000007000000}" name="eff_notes"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0A00-000008000000}" name="source"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0A00-000009000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="input_comm"/>
+    <tableColumn id="3" name="tech"/>
+    <tableColumn id="4" name="vintage"/>
+    <tableColumn id="5" name="output_comm"/>
+    <tableColumn id="6" name="efficiency"/>
+    <tableColumn id="7" name="eff_notes"/>
+    <tableColumn id="8" name="source"/>
+    <tableColumn id="9" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table12" displayName="Table12" ref="A1:K101" totalsRowShown="0">
-  <autoFilter ref="A1:K101" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="A1:K101" totalsRowShown="0">
+  <autoFilter ref="A1:K101"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="emis_comm"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="input_comm"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0B00-000004000000}" name="tech"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0B00-000005000000}" name="vintage"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0B00-000006000000}" name="output_comm"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0B00-000007000000}" name="emis_act"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0B00-000008000000}" name="emis_act_units"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0B00-000009000000}" name="emis_act_notes"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0B00-00000A000000}" name="source"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0B00-00000B000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="emis_comm"/>
+    <tableColumn id="3" name="input_comm"/>
+    <tableColumn id="4" name="tech"/>
+    <tableColumn id="5" name="vintage"/>
+    <tableColumn id="6" name="output_comm"/>
+    <tableColumn id="7" name="emis_act"/>
+    <tableColumn id="8" name="emis_act_units"/>
+    <tableColumn id="9" name="emis_act_notes"/>
+    <tableColumn id="10" name="source"/>
+    <tableColumn id="11" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Table13" displayName="Table13" ref="A1:H101" totalsRowShown="0">
-  <autoFilter ref="A1:H101" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="A1:H101" totalsRowShown="0">
+  <autoFilter ref="A1:H101"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="periods"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="emis_comm"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="emis_limit"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="emis_limit_units"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" name="emis_limit_notes"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" name="source"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0C00-000008000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="periods"/>
+    <tableColumn id="3" name="emis_comm"/>
+    <tableColumn id="4" name="emis_limit"/>
+    <tableColumn id="5" name="emis_limit_units"/>
+    <tableColumn id="6" name="emis_limit_notes"/>
+    <tableColumn id="7" name="source"/>
+    <tableColumn id="8" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table14" displayName="Table14" ref="A1:H101" totalsRowShown="0">
-  <autoFilter ref="A1:H101" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table14" displayName="Table14" ref="A1:H101" totalsRowShown="0">
+  <autoFilter ref="A1:H101"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="tech"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="vintage"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0D00-000004000000}" name="exist_cap"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0D00-000005000000}" name="exist_cap_units"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0D00-000006000000}" name="exist_cap_notes"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0D00-000007000000}" name="source"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0D00-000008000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="tech"/>
+    <tableColumn id="3" name="vintage"/>
+    <tableColumn id="4" name="exist_cap"/>
+    <tableColumn id="5" name="exist_cap_units"/>
+    <tableColumn id="6" name="exist_cap_notes"/>
+    <tableColumn id="7" name="source"/>
+    <tableColumn id="8" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Table15" displayName="Table15" ref="A1:C101" totalsRowShown="0">
-  <autoFilter ref="A1:C101" xr:uid="{00000000-0009-0000-0100-00000F000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table15" displayName="Table15" ref="A1:C101" totalsRowShown="0">
+  <autoFilter ref="A1:C101"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="rate"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="source"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="additional notes"/>
+    <tableColumn id="1" name="rate"/>
+    <tableColumn id="2" name="source"/>
+    <tableColumn id="3" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="Table16" displayName="Table16" ref="A1:F101" totalsRowShown="0">
-  <autoFilter ref="A1:F101" xr:uid="{00000000-0009-0000-0100-000010000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table16" displayName="Table16" ref="A1:F101" totalsRowShown="0">
+  <autoFilter ref="A1:F101"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="tech"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0F00-000003000000}" name="growthrate_max"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0F00-000004000000}" name="growthrate_max_notes"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0F00-000005000000}" name="source"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0F00-000006000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="tech"/>
+    <tableColumn id="3" name="growthrate_max"/>
+    <tableColumn id="4" name="growthrate_max_notes"/>
+    <tableColumn id="5" name="source"/>
+    <tableColumn id="6" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="Table17" displayName="Table17" ref="A1:G101" totalsRowShown="0">
-  <autoFilter ref="A1:G101" xr:uid="{00000000-0009-0000-0100-000011000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table17" displayName="Table17" ref="A1:G101" totalsRowShown="0">
+  <autoFilter ref="A1:G101"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="tech"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1000-000003000000}" name="growthrate_seed"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1000-000004000000}" name="growthrate_seed_units"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1000-000005000000}" name="growthrate_seed_notes"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1000-000006000000}" name="source"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1000-000007000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="tech"/>
+    <tableColumn id="3" name="growthrate_seed"/>
+    <tableColumn id="4" name="growthrate_seed_units"/>
+    <tableColumn id="5" name="growthrate_seed_notes"/>
+    <tableColumn id="6" name="source"/>
+    <tableColumn id="7" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="Table18" displayName="Table18" ref="A1:F101" totalsRowShown="0">
-  <autoFilter ref="A1:F101" xr:uid="{00000000-0009-0000-0100-000012000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table18" displayName="Table18" ref="A1:F101" totalsRowShown="0">
+  <autoFilter ref="A1:F101"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="tech"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1100-000003000000}" name="loan"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1100-000004000000}" name="loan_notes"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1100-000005000000}" name="source"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1100-000006000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="tech"/>
+    <tableColumn id="3" name="loan"/>
+    <tableColumn id="4" name="loan_notes"/>
+    <tableColumn id="5" name="source"/>
+    <tableColumn id="6" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF12000000}" name="Table19" displayName="Table19" ref="A1:G101" totalsRowShown="0">
-  <autoFilter ref="A1:G101" xr:uid="{00000000-0009-0000-0100-000013000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table19" displayName="Table19" ref="A1:G101" totalsRowShown="0">
+  <autoFilter ref="A1:G101"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1200-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1200-000002000000}" name="tech"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1200-000003000000}" name="vintage"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1200-000004000000}" name="life_process"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1200-000005000000}" name="life_process_notes"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1200-000006000000}" name="source"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1200-000007000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="tech"/>
+    <tableColumn id="3" name="vintage"/>
+    <tableColumn id="4" name="life_process"/>
+    <tableColumn id="5" name="life_process_notes"/>
+    <tableColumn id="6" name="source"/>
+    <tableColumn id="7" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:I101" totalsRowShown="0">
-  <autoFilter ref="A1:I101" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I101" totalsRowShown="0">
+  <autoFilter ref="A1:I101"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="season_name"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="time_of_day_name"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="tech"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="vintage"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="cf_process"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="cf_process_notes"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="source"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="season_name"/>
+    <tableColumn id="3" name="time_of_day_name"/>
+    <tableColumn id="4" name="tech"/>
+    <tableColumn id="5" name="vintage"/>
+    <tableColumn id="6" name="cf_process"/>
+    <tableColumn id="7" name="cf_process_notes"/>
+    <tableColumn id="8" name="source"/>
+    <tableColumn id="9" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{00000000-000C-0000-FFFF-FFFF13000000}" name="Table20" displayName="Table20" ref="A1:F101" totalsRowShown="0">
-  <autoFilter ref="A1:F101" xr:uid="{00000000-0009-0000-0100-000014000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table20" displayName="Table20" ref="A1:F101" totalsRowShown="0">
+  <autoFilter ref="A1:F101"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1300-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1300-000002000000}" name="tech"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1300-000003000000}" name="life"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1300-000004000000}" name="life_notes"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1300-000005000000}" name="source"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1300-000006000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="tech"/>
+    <tableColumn id="3" name="life"/>
+    <tableColumn id="4" name="life_notes"/>
+    <tableColumn id="5" name="source"/>
+    <tableColumn id="6" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{00000000-000C-0000-FFFF-FFFF14000000}" name="Table21" displayName="Table21" ref="A1:G101" totalsRowShown="0">
-  <autoFilter ref="A1:G101" xr:uid="{00000000-0009-0000-0100-000015000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table21" displayName="Table21" ref="A1:G101" totalsRowShown="0">
+  <autoFilter ref="A1:G101"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1400-000001000000}" name="primary_region"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1400-000002000000}" name="primary_tech"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1400-000003000000}" name="emis_comm"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1400-000004000000}" name="linked_tech"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1400-000005000000}" name="tech_linked_notes"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1400-000006000000}" name="source"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1400-000007000000}" name="additional notes"/>
+    <tableColumn id="1" name="primary_region"/>
+    <tableColumn id="2" name="primary_tech"/>
+    <tableColumn id="3" name="emis_comm"/>
+    <tableColumn id="4" name="linked_tech"/>
+    <tableColumn id="5" name="tech_linked_notes"/>
+    <tableColumn id="6" name="source"/>
+    <tableColumn id="7" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{00000000-000C-0000-FFFF-FFFF15000000}" name="Table22" displayName="Table22" ref="A1:H101" totalsRowShown="0">
-  <autoFilter ref="A1:H101" xr:uid="{00000000-0009-0000-0100-000016000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Table22" displayName="Table22" ref="A1:H101" totalsRowShown="0">
+  <autoFilter ref="A1:H101"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1500-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1500-000002000000}" name="periods"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1500-000003000000}" name="tech"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1500-000004000000}" name="maxact"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1500-000005000000}" name="maxact_units"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1500-000006000000}" name="maxact_notes"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1500-000007000000}" name="source"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1500-000008000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="periods"/>
+    <tableColumn id="3" name="tech"/>
+    <tableColumn id="4" name="maxact"/>
+    <tableColumn id="5" name="maxact_units"/>
+    <tableColumn id="6" name="maxact_notes"/>
+    <tableColumn id="7" name="source"/>
+    <tableColumn id="8" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{00000000-000C-0000-FFFF-FFFF16000000}" name="Table23" displayName="Table23" ref="A1:H101" totalsRowShown="0">
-  <autoFilter ref="A1:H101" xr:uid="{00000000-0009-0000-0100-000017000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Table23" displayName="Table23" ref="A1:H101" totalsRowShown="0">
+  <autoFilter ref="A1:H101"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1600-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1600-000002000000}" name="periods"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1600-000003000000}" name="tech"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1600-000004000000}" name="maxcap"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1600-000005000000}" name="maxcap_units"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1600-000006000000}" name="maxcap_notes"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1600-000007000000}" name="source"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1600-000008000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="periods"/>
+    <tableColumn id="3" name="tech"/>
+    <tableColumn id="4" name="maxcap"/>
+    <tableColumn id="5" name="maxcap_units"/>
+    <tableColumn id="6" name="maxcap_notes"/>
+    <tableColumn id="7" name="source"/>
+    <tableColumn id="8" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{00000000-000C-0000-FFFF-FFFF17000000}" name="Table24" displayName="Table24" ref="A1:G101" totalsRowShown="0">
-  <autoFilter ref="A1:G101" xr:uid="{00000000-0009-0000-0100-000018000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Table24" displayName="Table24" ref="A1:G101" totalsRowShown="0">
+  <autoFilter ref="A1:G101"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1700-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1700-000002000000}" name="tech"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1700-000003000000}" name="maxres"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1700-000004000000}" name="maxres_units"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1700-000005000000}" name="maxres_notes"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1700-000006000000}" name="source"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1700-000007000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="tech"/>
+    <tableColumn id="3" name="maxres"/>
+    <tableColumn id="4" name="maxres_units"/>
+    <tableColumn id="5" name="maxres_notes"/>
+    <tableColumn id="6" name="source"/>
+    <tableColumn id="7" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{00000000-000C-0000-FFFF-FFFF18000000}" name="Table25" displayName="Table25" ref="A1:H101" totalsRowShown="0">
-  <autoFilter ref="A1:H101" xr:uid="{00000000-0009-0000-0100-000019000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Table25" displayName="Table25" ref="A1:H101" totalsRowShown="0">
+  <autoFilter ref="A1:H101"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1800-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1800-000002000000}" name="periods"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1800-000003000000}" name="tech"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1800-000004000000}" name="minact"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1800-000005000000}" name="minact_units"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1800-000006000000}" name="minact_notes"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1800-000007000000}" name="source"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1800-000008000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="periods"/>
+    <tableColumn id="3" name="tech"/>
+    <tableColumn id="4" name="minact"/>
+    <tableColumn id="5" name="minact_units"/>
+    <tableColumn id="6" name="minact_notes"/>
+    <tableColumn id="7" name="source"/>
+    <tableColumn id="8" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{00000000-000C-0000-FFFF-FFFF19000000}" name="Table26" displayName="Table26" ref="A1:H101" totalsRowShown="0">
-  <autoFilter ref="A1:H101" xr:uid="{00000000-0009-0000-0100-00001A000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Table26" displayName="Table26" ref="A1:H101" totalsRowShown="0">
+  <autoFilter ref="A1:H101"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1900-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1900-000002000000}" name="periods"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1900-000003000000}" name="tech"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1900-000004000000}" name="mincap"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1900-000005000000}" name="mincap_units"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1900-000006000000}" name="mincap_notes"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1900-000007000000}" name="source"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1900-000008000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="periods"/>
+    <tableColumn id="3" name="tech"/>
+    <tableColumn id="4" name="mincap"/>
+    <tableColumn id="5" name="mincap_units"/>
+    <tableColumn id="6" name="mincap_notes"/>
+    <tableColumn id="7" name="source"/>
+    <tableColumn id="8" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{00000000-000C-0000-FFFF-FFFF1A000000}" name="Table27" displayName="Table27" ref="A1:G101" totalsRowShown="0">
-  <autoFilter ref="A1:G101" xr:uid="{00000000-0009-0000-0100-00001B000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="Table27" displayName="Table27" ref="A1:G101" totalsRowShown="0">
+  <autoFilter ref="A1:G101"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1A00-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1A00-000002000000}" name="periods"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1A00-000003000000}" name="group_name"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1A00-000004000000}" name="min_act_g"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1A00-000005000000}" name="notes"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1A00-000006000000}" name="source"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1A00-000007000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="periods"/>
+    <tableColumn id="3" name="group_name"/>
+    <tableColumn id="4" name="min_act_g"/>
+    <tableColumn id="5" name="notes"/>
+    <tableColumn id="6" name="source"/>
+    <tableColumn id="7" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{00000000-000C-0000-FFFF-FFFF1B000000}" name="Table28" displayName="Table28" ref="A1:G101" totalsRowShown="0">
-  <autoFilter ref="A1:G101" xr:uid="{00000000-0009-0000-0100-00001C000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Table28" displayName="Table28" ref="A1:G101" totalsRowShown="0">
+  <autoFilter ref="A1:G101"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1B00-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1B00-000002000000}" name="tech"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1B00-000003000000}" name="group_name"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1B00-000004000000}" name="act_fraction"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1B00-000005000000}" name="tech_desc"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1B00-000006000000}" name="source"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1B00-000007000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="tech"/>
+    <tableColumn id="3" name="group_name"/>
+    <tableColumn id="4" name="act_fraction"/>
+    <tableColumn id="5" name="tech_desc"/>
+    <tableColumn id="6" name="source"/>
+    <tableColumn id="7" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{00000000-000C-0000-FFFF-FFFF1C000000}" name="Table29" displayName="Table29" ref="A1:C101" totalsRowShown="0">
-  <autoFilter ref="A1:C101" xr:uid="{00000000-0009-0000-0100-00001D000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Table29" displayName="Table29" ref="A1:C101" totalsRowShown="0">
+  <autoFilter ref="A1:C101"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1C00-000001000000}" name="year"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1C00-000002000000}" name="source"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1C00-000003000000}" name="additional notes"/>
+    <tableColumn id="1" name="year"/>
+    <tableColumn id="2" name="source"/>
+    <tableColumn id="3" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A1:H101" totalsRowShown="0">
-  <autoFilter ref="A1:H101" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:H101" totalsRowShown="0">
+  <autoFilter ref="A1:H101"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="season_name"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="time_of_day_name"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="tech"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="cf_tech"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="cf_tech_notes"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="source"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="season_name"/>
+    <tableColumn id="3" name="time_of_day_name"/>
+    <tableColumn id="4" name="tech"/>
+    <tableColumn id="5" name="cf_tech"/>
+    <tableColumn id="6" name="cf_tech_notes"/>
+    <tableColumn id="7" name="source"/>
+    <tableColumn id="8" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{00000000-000C-0000-FFFF-FFFF1D000000}" name="Table30" displayName="Table30" ref="A1:D101" totalsRowShown="0">
-  <autoFilter ref="A1:D101" xr:uid="{00000000-0009-0000-0100-00001E000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="Table30" displayName="Table30" ref="A1:D101" totalsRowShown="0">
+  <autoFilter ref="A1:D101"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1D00-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1D00-000002000000}" name="reserve_margin"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1D00-000003000000}" name="source"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1D00-000004000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="reserve_margin"/>
+    <tableColumn id="3" name="source"/>
+    <tableColumn id="4" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{00000000-000C-0000-FFFF-FFFF1E000000}" name="Table31" displayName="Table31" ref="A1:E101" totalsRowShown="0">
-  <autoFilter ref="A1:E101" xr:uid="{00000000-0009-0000-0100-00001F000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Table31" displayName="Table31" ref="A1:E101" totalsRowShown="0">
+  <autoFilter ref="A1:E101"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1E00-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1E00-000002000000}" name="tech"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1E00-000003000000}" name="ramp_down"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1E00-000004000000}" name="source"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1E00-000005000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="tech"/>
+    <tableColumn id="3" name="ramp_down"/>
+    <tableColumn id="4" name="source"/>
+    <tableColumn id="5" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{00000000-000C-0000-FFFF-FFFF1F000000}" name="Table32" displayName="Table32" ref="A1:E101" totalsRowShown="0">
-  <autoFilter ref="A1:E101" xr:uid="{00000000-0009-0000-0100-000020000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="32" name="Table32" displayName="Table32" ref="A1:E101" totalsRowShown="0">
+  <autoFilter ref="A1:E101"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1F00-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1F00-000002000000}" name="tech"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1F00-000003000000}" name="ramp_up"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1F00-000004000000}" name="source"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1F00-000005000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="tech"/>
+    <tableColumn id="3" name="ramp_up"/>
+    <tableColumn id="4" name="source"/>
+    <tableColumn id="5" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table33.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{00000000-000C-0000-FFFF-FFFF20000000}" name="Table33" displayName="Table33" ref="A1:F101" totalsRowShown="0">
-  <autoFilter ref="A1:F101" xr:uid="{00000000-0009-0000-0100-000021000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="33" name="Table33" displayName="Table33" ref="A1:F101" totalsRowShown="0">
+  <autoFilter ref="A1:F101"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2000-000001000000}" name="season_name"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2000-000002000000}" name="time_of_day_name"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2000-000003000000}" name="segfrac"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2000-000004000000}" name="segfrac_notes"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2000-000005000000}" name="source"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2000-000006000000}" name="additional notes"/>
+    <tableColumn id="1" name="season_name"/>
+    <tableColumn id="2" name="time_of_day_name"/>
+    <tableColumn id="3" name="segfrac"/>
+    <tableColumn id="4" name="segfrac_notes"/>
+    <tableColumn id="5" name="source"/>
+    <tableColumn id="6" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table34.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{00000000-000C-0000-FFFF-FFFF21000000}" name="Table34" displayName="Table34" ref="A1:F101" totalsRowShown="0">
-  <autoFilter ref="A1:F101" xr:uid="{00000000-0009-0000-0100-000022000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="34" name="Table34" displayName="Table34" ref="A1:F101" totalsRowShown="0">
+  <autoFilter ref="A1:F101"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2100-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2100-000002000000}" name="tech"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2100-000003000000}" name="duration"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2100-000004000000}" name="duration_notes"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2100-000005000000}" name="source"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2100-000006000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="tech"/>
+    <tableColumn id="3" name="duration"/>
+    <tableColumn id="4" name="duration_notes"/>
+    <tableColumn id="5" name="source"/>
+    <tableColumn id="6" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table35.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{00000000-000C-0000-FFFF-FFFF22000000}" name="Table35" displayName="Table35" ref="A1:H101" totalsRowShown="0">
-  <autoFilter ref="A1:H101" xr:uid="{00000000-0009-0000-0100-000023000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="35" name="Table35" displayName="Table35" ref="A1:H101" totalsRowShown="0">
+  <autoFilter ref="A1:H101"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2200-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2200-000002000000}" name="periods"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2200-000003000000}" name="input_comm"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2200-000004000000}" name="tech"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2200-000005000000}" name="ti_split"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2200-000006000000}" name="ti_split_notes"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-2200-000007000000}" name="source"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-2200-000008000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="periods"/>
+    <tableColumn id="3" name="input_comm"/>
+    <tableColumn id="4" name="tech"/>
+    <tableColumn id="5" name="ti_split"/>
+    <tableColumn id="6" name="ti_split_notes"/>
+    <tableColumn id="7" name="source"/>
+    <tableColumn id="8" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table36.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="36" xr:uid="{00000000-000C-0000-FFFF-FFFF23000000}" name="Table36" displayName="Table36" ref="A1:H101" totalsRowShown="0">
-  <autoFilter ref="A1:H101" xr:uid="{00000000-0009-0000-0100-000024000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="36" name="Table36" displayName="Table36" ref="A1:H101" totalsRowShown="0">
+  <autoFilter ref="A1:H101"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2300-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2300-000002000000}" name="periods"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2300-000003000000}" name="input_comm"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2300-000004000000}" name="tech"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2300-000005000000}" name="ti_split"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2300-000006000000}" name="ti_split_notes"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-2300-000007000000}" name="source"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-2300-000008000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="periods"/>
+    <tableColumn id="3" name="input_comm"/>
+    <tableColumn id="4" name="tech"/>
+    <tableColumn id="5" name="ti_split"/>
+    <tableColumn id="6" name="ti_split_notes"/>
+    <tableColumn id="7" name="source"/>
+    <tableColumn id="8" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table37.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="37" xr:uid="{00000000-000C-0000-FFFF-FFFF24000000}" name="Table37" displayName="Table37" ref="A1:H101" totalsRowShown="0">
-  <autoFilter ref="A1:H101" xr:uid="{00000000-0009-0000-0100-000025000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="37" name="Table37" displayName="Table37" ref="A1:H101" totalsRowShown="0">
+  <autoFilter ref="A1:H101"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2400-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2400-000002000000}" name="periods"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2400-000003000000}" name="tech"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2400-000004000000}" name="output_comm"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2400-000005000000}" name="to_split"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2400-000006000000}" name="to_split_notes"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-2400-000007000000}" name="source"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-2400-000008000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="periods"/>
+    <tableColumn id="3" name="tech"/>
+    <tableColumn id="4" name="output_comm"/>
+    <tableColumn id="5" name="to_split"/>
+    <tableColumn id="6" name="to_split_notes"/>
+    <tableColumn id="7" name="source"/>
+    <tableColumn id="8" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table38.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="38" xr:uid="{00000000-000C-0000-FFFF-FFFF25000000}" name="Table38" displayName="Table38" ref="A1:E101" totalsRowShown="0">
-  <autoFilter ref="A1:E101" xr:uid="{00000000-0009-0000-0100-000026000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="38" name="Table38" displayName="Table38" ref="A1:E101" totalsRowShown="0">
+  <autoFilter ref="A1:E101"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2500-000001000000}" name="comm_name"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2500-000002000000}" name="flag"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2500-000003000000}" name="comm_desc"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2500-000004000000}" name="source"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2500-000005000000}" name="additional notes"/>
+    <tableColumn id="1" name="comm_name"/>
+    <tableColumn id="2" name="flag"/>
+    <tableColumn id="3" name="comm_desc"/>
+    <tableColumn id="4" name="source"/>
+    <tableColumn id="5" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table39.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="39" xr:uid="{00000000-000C-0000-FFFF-FFFF26000000}" name="Table39" displayName="Table39" ref="A1:D101" totalsRowShown="0">
-  <autoFilter ref="A1:D101" xr:uid="{00000000-0009-0000-0100-000027000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="39" name="Table39" displayName="Table39" ref="A1:D101" totalsRowShown="0">
+  <autoFilter ref="A1:D101"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2600-000001000000}" name="comm_labels"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2600-000002000000}" name="comm_labels_desc"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2600-000003000000}" name="source"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2600-000004000000}" name="additional notes"/>
+    <tableColumn id="1" name="comm_labels"/>
+    <tableColumn id="2" name="comm_labels_desc"/>
+    <tableColumn id="3" name="source"/>
+    <tableColumn id="4" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table4" displayName="Table4" ref="A1:F101" totalsRowShown="0">
-  <autoFilter ref="A1:F101" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:F101" totalsRowShown="0">
+  <autoFilter ref="A1:F101"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="tech"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="c2a"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="c2a_notes"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="source"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="tech"/>
+    <tableColumn id="3" name="c2a"/>
+    <tableColumn id="4" name="c2a_notes"/>
+    <tableColumn id="5" name="source"/>
+    <tableColumn id="6" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table40.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="40" xr:uid="{00000000-000C-0000-FFFF-FFFF27000000}" name="Table40" displayName="Table40" ref="A1:D101" totalsRowShown="0">
-  <autoFilter ref="A1:D101" xr:uid="{00000000-0009-0000-0100-000028000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="40" name="Table40" displayName="Table40" ref="A1:D101" totalsRowShown="0">
+  <autoFilter ref="A1:D101"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2700-000001000000}" name="group_name"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2700-000002000000}" name="notes"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2700-000003000000}" name="source"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2700-000004000000}" name="additional notes"/>
+    <tableColumn id="1" name="group_name"/>
+    <tableColumn id="2" name="notes"/>
+    <tableColumn id="3" name="source"/>
+    <tableColumn id="4" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table41.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="41" xr:uid="{00000000-000C-0000-FFFF-FFFF28000000}" name="Table41" displayName="Table41" ref="A1:D101" totalsRowShown="0">
-  <autoFilter ref="A1:D101" xr:uid="{00000000-0009-0000-0100-000029000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="41" name="Table41" displayName="Table41" ref="A1:D101" totalsRowShown="0">
+  <autoFilter ref="A1:D101"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2800-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2800-000002000000}" name="region_note"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2800-000003000000}" name="source"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2800-000004000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="region_note"/>
+    <tableColumn id="3" name="source"/>
+    <tableColumn id="4" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table42.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="42" xr:uid="{00000000-000C-0000-FFFF-FFFF29000000}" name="Table42" displayName="Table42" ref="A1:C101" totalsRowShown="0">
-  <autoFilter ref="A1:C101" xr:uid="{00000000-0009-0000-0100-00002A000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="42" name="Table42" displayName="Table42" ref="A1:C101" totalsRowShown="0">
+  <autoFilter ref="A1:C101"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2900-000001000000}" name="sector"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2900-000002000000}" name="source"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2900-000003000000}" name="additional notes"/>
+    <tableColumn id="1" name="sector"/>
+    <tableColumn id="2" name="source"/>
+    <tableColumn id="3" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table43.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="43" xr:uid="{00000000-000C-0000-FFFF-FFFF2A000000}" name="Table43" displayName="Table43" ref="A1:D101" totalsRowShown="0">
-  <autoFilter ref="A1:D101" xr:uid="{00000000-0009-0000-0100-00002B000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="43" name="Table43" displayName="Table43" ref="A1:D101" totalsRowShown="0">
+  <autoFilter ref="A1:D101"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2A00-000001000000}" name="tech"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2A00-000002000000}" name="notes"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2A00-000003000000}" name="source"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2A00-000004000000}" name="additional notes"/>
+    <tableColumn id="1" name="tech"/>
+    <tableColumn id="2" name="notes"/>
+    <tableColumn id="3" name="source"/>
+    <tableColumn id="4" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table44.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="44" xr:uid="{00000000-000C-0000-FFFF-FFFF2B000000}" name="Table44" displayName="Table44" ref="A1:D101" totalsRowShown="0">
-  <autoFilter ref="A1:D101" xr:uid="{00000000-0009-0000-0100-00002C000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="44" name="Table44" displayName="Table44" ref="A1:D101" totalsRowShown="0">
+  <autoFilter ref="A1:D101"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2B00-000001000000}" name="tech"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2B00-000002000000}" name="notes"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2B00-000003000000}" name="source"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2B00-000004000000}" name="additional notes"/>
+    <tableColumn id="1" name="tech"/>
+    <tableColumn id="2" name="notes"/>
+    <tableColumn id="3" name="source"/>
+    <tableColumn id="4" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table45.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="45" xr:uid="{00000000-000C-0000-FFFF-FFFF2C000000}" name="Table45" displayName="Table45" ref="A1:D101" totalsRowShown="0">
-  <autoFilter ref="A1:D101" xr:uid="{00000000-0009-0000-0100-00002D000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="45" name="Table45" displayName="Table45" ref="A1:D101" totalsRowShown="0">
+  <autoFilter ref="A1:D101"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2C00-000001000000}" name="tech"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2C00-000002000000}" name="notes"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2C00-000003000000}" name="source"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2C00-000004000000}" name="additional notes"/>
+    <tableColumn id="1" name="tech"/>
+    <tableColumn id="2" name="notes"/>
+    <tableColumn id="3" name="source"/>
+    <tableColumn id="4" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table46.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="46" xr:uid="{00000000-000C-0000-FFFF-FFFF2D000000}" name="Table46" displayName="Table46" ref="A1:D101" totalsRowShown="0">
-  <autoFilter ref="A1:D101" xr:uid="{00000000-0009-0000-0100-00002E000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="46" name="Table46" displayName="Table46" ref="A1:D101" totalsRowShown="0">
+  <autoFilter ref="A1:D101"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2D00-000001000000}" name="tech"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2D00-000002000000}" name="notes"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2D00-000003000000}" name="source"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2D00-000004000000}" name="additional notes"/>
+    <tableColumn id="1" name="tech"/>
+    <tableColumn id="2" name="notes"/>
+    <tableColumn id="3" name="source"/>
+    <tableColumn id="4" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table47.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="47" xr:uid="{00000000-000C-0000-FFFF-FFFF2E000000}" name="Table47" displayName="Table47" ref="A1:C101" totalsRowShown="0">
-  <autoFilter ref="A1:C101" xr:uid="{00000000-0009-0000-0100-00002F000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="47" name="Table47" displayName="Table47" ref="A1:C101" totalsRowShown="0">
+  <autoFilter ref="A1:C101"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2E00-000001000000}" name="tech"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2E00-000002000000}" name="source"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2E00-000003000000}" name="additional notes"/>
+    <tableColumn id="1" name="tech"/>
+    <tableColumn id="2" name="source"/>
+    <tableColumn id="3" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table48.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="48" xr:uid="{00000000-000C-0000-FFFF-FFFF2F000000}" name="Table48" displayName="Table48" ref="A1:D101" totalsRowShown="0">
-  <autoFilter ref="A1:D101" xr:uid="{00000000-0009-0000-0100-000030000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="48" name="Table48" displayName="Table48" ref="A1:D101" totalsRowShown="0">
+  <autoFilter ref="A1:D101"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2F00-000001000000}" name="tech"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2F00-000002000000}" name="notes"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2F00-000003000000}" name="source"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2F00-000004000000}" name="additional notes"/>
+    <tableColumn id="1" name="tech"/>
+    <tableColumn id="2" name="notes"/>
+    <tableColumn id="3" name="source"/>
+    <tableColumn id="4" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table49.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="49" xr:uid="{00000000-000C-0000-FFFF-FFFF30000000}" name="Table49" displayName="Table49" ref="A1:G101" totalsRowShown="0">
-  <autoFilter ref="A1:G101" xr:uid="{00000000-0009-0000-0100-000031000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="49" name="Table49" displayName="Table49" ref="A1:G101" totalsRowShown="0">
+  <autoFilter ref="A1:G101"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-3000-000001000000}" name="tech"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-3000-000002000000}" name="flag"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-3000-000003000000}" name="sector"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-3000-000004000000}" name="tech_desc"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-3000-000005000000}" name="tech_category"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-3000-000006000000}" name="source"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-3000-000007000000}" name="additional notes"/>
+    <tableColumn id="1" name="tech"/>
+    <tableColumn id="2" name="flag"/>
+    <tableColumn id="3" name="sector"/>
+    <tableColumn id="4" name="tech_desc"/>
+    <tableColumn id="5" name="tech_category"/>
+    <tableColumn id="6" name="source"/>
+    <tableColumn id="7" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table5" displayName="Table5" ref="A1:I101" totalsRowShown="0">
-  <autoFilter ref="A1:I101" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:I101" totalsRowShown="0">
+  <autoFilter ref="A1:I101"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="periods"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="tech"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="vintage"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="cost_fixed"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="cost_fixed_units"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="cost_fixed_notes"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="source"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="periods"/>
+    <tableColumn id="3" name="tech"/>
+    <tableColumn id="4" name="vintage"/>
+    <tableColumn id="5" name="cost_fixed"/>
+    <tableColumn id="6" name="cost_fixed_units"/>
+    <tableColumn id="7" name="cost_fixed_notes"/>
+    <tableColumn id="8" name="source"/>
+    <tableColumn id="9" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table50.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="50" xr:uid="{00000000-000C-0000-FFFF-FFFF31000000}" name="Table50" displayName="Table50" ref="A1:D101" totalsRowShown="0">
-  <autoFilter ref="A1:D101" xr:uid="{00000000-0009-0000-0100-000032000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="50" name="Table50" displayName="Table50" ref="A1:D101" totalsRowShown="0">
+  <autoFilter ref="A1:D101"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-3100-000001000000}" name="tech_labels"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-3100-000002000000}" name="tech_labels_desc"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-3100-000003000000}" name="source"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-3100-000004000000}" name="additional notes"/>
+    <tableColumn id="1" name="tech_labels"/>
+    <tableColumn id="2" name="tech_labels_desc"/>
+    <tableColumn id="3" name="source"/>
+    <tableColumn id="4" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table51.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="51" xr:uid="{00000000-000C-0000-FFFF-FFFF32000000}" name="Table51" displayName="Table51" ref="A1:C101" totalsRowShown="0">
-  <autoFilter ref="A1:C101" xr:uid="{00000000-0009-0000-0100-000033000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="51" name="Table51" displayName="Table51" ref="A1:C101" totalsRowShown="0">
+  <autoFilter ref="A1:C101"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-3200-000001000000}" name="t_day"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-3200-000002000000}" name="source"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-3200-000003000000}" name="additional notes"/>
+    <tableColumn id="1" name="t_day"/>
+    <tableColumn id="2" name="source"/>
+    <tableColumn id="3" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table52.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="52" xr:uid="{00000000-000C-0000-FFFF-FFFF33000000}" name="Table52" displayName="Table52" ref="A1:D101" totalsRowShown="0">
-  <autoFilter ref="A1:D101" xr:uid="{00000000-0009-0000-0100-000034000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="52" name="Table52" displayName="Table52" ref="A1:D101" totalsRowShown="0">
+  <autoFilter ref="A1:D101"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-3300-000001000000}" name="t_period_labels"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-3300-000002000000}" name="t_period_labels_desc"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-3300-000003000000}" name="source"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-3300-000004000000}" name="additional notes"/>
+    <tableColumn id="1" name="t_period_labels"/>
+    <tableColumn id="2" name="t_period_labels_desc"/>
+    <tableColumn id="3" name="source"/>
+    <tableColumn id="4" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table53.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="53" xr:uid="{00000000-000C-0000-FFFF-FFFF34000000}" name="Table53" displayName="Table53" ref="A1:D101" totalsRowShown="0">
-  <autoFilter ref="A1:D101" xr:uid="{00000000-0009-0000-0100-000035000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="53" name="Table53" displayName="Table53" ref="A1:D101" totalsRowShown="0">
+  <autoFilter ref="A1:D101"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-3400-000001000000}" name="t_periods"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-3400-000002000000}" name="flag"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-3400-000003000000}" name="source"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-3400-000004000000}" name="additional notes"/>
+    <tableColumn id="1" name="t_periods"/>
+    <tableColumn id="2" name="flag"/>
+    <tableColumn id="3" name="source"/>
+    <tableColumn id="4" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table54.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="54" xr:uid="{00000000-000C-0000-FFFF-FFFF35000000}" name="Table54" displayName="Table54" ref="A1:C101" totalsRowShown="0">
-  <autoFilter ref="A1:C101" xr:uid="{00000000-0009-0000-0100-000036000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="54" name="Table54" displayName="Table54" ref="A1:C101" totalsRowShown="0">
+  <autoFilter ref="A1:C101"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-3500-000001000000}" name="t_season"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-3500-000002000000}" name="source"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-3500-000003000000}" name="additional notes"/>
+    <tableColumn id="1" name="t_season"/>
+    <tableColumn id="2" name="source"/>
+    <tableColumn id="3" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table6" displayName="Table6" ref="A1:H101" totalsRowShown="0">
-  <autoFilter ref="A1:H101" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:H101" totalsRowShown="0">
+  <autoFilter ref="A1:H101"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="tech"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="vintage"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="cost_invest"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="cost_invest_units"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="cost_invest_notes"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="source"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="tech"/>
+    <tableColumn id="3" name="vintage"/>
+    <tableColumn id="4" name="cost_invest"/>
+    <tableColumn id="5" name="cost_invest_units"/>
+    <tableColumn id="6" name="cost_invest_notes"/>
+    <tableColumn id="7" name="source"/>
+    <tableColumn id="8" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table7" displayName="Table7" ref="A1:I101" totalsRowShown="0">
-  <autoFilter ref="A1:I101" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:I101" totalsRowShown="0">
+  <autoFilter ref="A1:I101"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="periods"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="tech"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="vintage"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="cost_variable"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="cost_variable_units"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="cost_variable_notes"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="source"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="periods"/>
+    <tableColumn id="3" name="tech"/>
+    <tableColumn id="4" name="vintage"/>
+    <tableColumn id="5" name="cost_variable"/>
+    <tableColumn id="6" name="cost_variable_units"/>
+    <tableColumn id="7" name="cost_variable_notes"/>
+    <tableColumn id="8" name="source"/>
+    <tableColumn id="9" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table8" displayName="Table8" ref="A1:H101" totalsRowShown="0">
-  <autoFilter ref="A1:H101" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:H101" totalsRowShown="0">
+  <autoFilter ref="A1:H101"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="periods"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="demand_comm"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="demand"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="demand_units"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="demand_notes"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="source"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="periods"/>
+    <tableColumn id="3" name="demand_comm"/>
+    <tableColumn id="4" name="demand"/>
+    <tableColumn id="5" name="demand_units"/>
+    <tableColumn id="6" name="demand_notes"/>
+    <tableColumn id="7" name="source"/>
+    <tableColumn id="8" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table9" displayName="Table9" ref="A1:H101" totalsRowShown="0">
-  <autoFilter ref="A1:H101" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A1:H101" totalsRowShown="0">
+  <autoFilter ref="A1:H101"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="regions"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="season_name"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="time_of_day_name"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="demand_name"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="dds"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="dds_notes"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="source"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="additional notes"/>
+    <tableColumn id="1" name="regions"/>
+    <tableColumn id="2" name="season_name"/>
+    <tableColumn id="3" name="time_of_day_name"/>
+    <tableColumn id="4" name="demand_name"/>
+    <tableColumn id="5" name="dds"/>
+    <tableColumn id="6" name="dds_notes"/>
+    <tableColumn id="7" name="source"/>
+    <tableColumn id="8" name="additional notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1315,7 +1301,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1347,27 +1333,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1399,24 +1367,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1592,17 +1542,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="8" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="8" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1637,17 +1588,18 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="7" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="7" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1679,17 +1631,18 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="9" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="9" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1727,17 +1680,18 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="11" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="11" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1781,17 +1735,18 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="8" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="8" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1826,17 +1781,18 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="8" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="8" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1871,17 +1827,18 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="3" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="3" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -1901,17 +1858,18 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="6" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="6" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1940,17 +1898,18 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="7" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="7" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1982,17 +1941,18 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="6" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="6" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2021,17 +1981,18 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="7" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="7" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2063,17 +2024,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="9" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="9" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2111,17 +2073,18 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="6" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="6" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2150,17 +2113,18 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="7" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="7" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -2192,17 +2156,18 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="8" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="8" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2237,17 +2202,18 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="8" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="8" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2282,17 +2248,18 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="7" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="7" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2324,17 +2291,18 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="8" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="8" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2369,17 +2337,18 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="8" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="8" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2414,17 +2383,18 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="7" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="7" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2456,17 +2426,18 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="7" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="7" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2498,17 +2469,18 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="3" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="3" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>82</v>
       </c>
@@ -2528,17 +2500,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="8" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="8" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2573,200 +2546,206 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="4" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="5" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="5" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="4" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <col min="5" max="6" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="6" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="5" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
+        <v>88</v>
+      </c>
+      <c r="D1" t="s">
+        <v>89</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="5" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="6" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="6" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="8" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <col min="7" max="8" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2801,17 +2780,18 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="8" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="8" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2846,17 +2826,18 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="8" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="8" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2891,416 +2872,429 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="5" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="4" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="6" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="4" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="4" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="3" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="4" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="4" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="4" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="4" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="3" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="4" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="5" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="4" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="6" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="4" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="4" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="3" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="4" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="4" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="4" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="4" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="3" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="4" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="7" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <col min="6" max="7" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -3332,17 +3326,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="9" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="9" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3380,17 +3375,18 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="4" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="4" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>102</v>
       </c>
@@ -3413,17 +3409,18 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="3" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="3" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>104</v>
       </c>
@@ -3443,17 +3440,18 @@
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="4" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="4" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>105</v>
       </c>
@@ -3476,17 +3474,18 @@
 </file>
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="4" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="4" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>107</v>
       </c>
@@ -3509,17 +3508,18 @@
 </file>
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="3" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="3" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>108</v>
       </c>
@@ -3539,17 +3539,18 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="8" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="8" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3584,17 +3585,18 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="9" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="9" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3632,19 +3634,18 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="8" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="8" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3679,17 +3680,18 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="8" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="8" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>